<commit_message>
start building model changes
</commit_message>
<xml_diff>
--- a/tests/resources/Light Vehicles for VTM.xlsx
+++ b/tests/resources/Light Vehicles for VTM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven.Pears/Documents/GitHub/cvs-tsk-lgv-file-import/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE88498-9C08-FB47-AC8F-B5B76073704B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DED41D6-551F-A54D-AB6D-F340C78E5C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{B1A1485B-1367-4AFC-8CDA-94A3C9038D55}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{B1A1485B-1367-4AFC-8CDA-94A3C9038D55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Vehicle Identification Number (VIN)</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Vehicle Registration Mark (VRM) \ Z number</t>
   </si>
   <si>
-    <t>1234Z</t>
-  </si>
-  <si>
     <t>N, P, A, S, C, L, T, E, M , R, W</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>Bike, bike and sidecar, trike or quad</t>
   </si>
   <si>
-    <t>150cc</t>
-  </si>
-  <si>
     <t>Vehicle Class (for IVA only)</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
   </si>
   <si>
     <t>sidecar</t>
-  </si>
-  <si>
-    <t>1500cc</t>
   </si>
 </sst>
 </file>
@@ -519,7 +510,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -535,7 +526,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -547,59 +538,57 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4">
         <v>123456</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="G2" s="4">
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>19</v>
+      <c r="G3" s="7">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update lambda service test
</commit_message>
<xml_diff>
--- a/tests/resources/Light Vehicles for VTM.xlsx
+++ b/tests/resources/Light Vehicles for VTM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven.Pears/Documents/GitHub/cvs-tsk-lgv-file-import/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DED41D6-551F-A54D-AB6D-F340C78E5C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BA85BE-AB41-EF4E-9E87-381525B2FF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{B1A1485B-1367-4AFC-8CDA-94A3C9038D55}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>Engine CC (for MSVA only)</t>
   </si>
   <si>
-    <t>Tweet</t>
-  </si>
-  <si>
     <t>ABCDEF</t>
   </si>
   <si>
@@ -87,13 +84,16 @@
   </si>
   <si>
     <t>sidecar</t>
+  </si>
+  <si>
+    <t>PSMVA1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +124,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -167,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -193,6 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,7 +517,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -569,23 +576,23 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="G3" s="7">
         <v>1500</v>

</xml_diff>